<commit_message>
end of single stim messurements
</commit_message>
<xml_diff>
--- a/Training_Messreihe.xlsx
+++ b/Training_Messreihe.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="55"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="12.08.2021" sheetId="1" state="visible" r:id="rId2"/>
@@ -569,7 +569,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -7872,12 +7872,13 @@
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
@@ -15153,7 +15154,7 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -22304,7 +22305,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
@@ -22740,11 +22741,11 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">

</xml_diff>

<commit_message>
major typo found in origin data, trying to get the boxplots. vertical lines for different messuring phases added
</commit_message>
<xml_diff>
--- a/Training_Messreihe.xlsx
+++ b/Training_Messreihe.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="57"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="12.08.2021" sheetId="1" state="visible" r:id="rId2"/>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="13">
   <si>
     <t xml:space="preserve">Seite</t>
   </si>
@@ -188,16 +188,13 @@
     <t xml:space="preserve">left</t>
   </si>
   <si>
-    <t xml:space="preserve">2021albi02</t>
+    <t xml:space="preserve">2020albi02</t>
   </si>
   <si>
     <t xml:space="preserve">2020albi03</t>
   </si>
   <si>
     <t xml:space="preserve">2020albi01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020albi02</t>
   </si>
   <si>
     <t xml:space="preserve">01. + </t>
@@ -606,7 +603,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+      <selection pane="topLeft" activeCell="J27" activeCellId="1" sqref="I16:I18 J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1218,7 +1215,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="I16:I18 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1237,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
@@ -1949,7 +1946,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="1" sqref="I16:I18 C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2508,7 +2505,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="1" sqref="I16:I18 C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2911,7 +2908,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2930,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>10</v>
@@ -3313,7 +3310,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3329,7 +3326,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>10</v>
@@ -3980,7 +3977,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4005,7 +4002,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4287,7 +4284,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="I16:I18 C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4586,7 +4583,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4608,7 +4605,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4882,7 +4879,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="I16:I18 C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4892,7 +4889,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
@@ -5181,7 +5178,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5203,7 +5200,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5480,7 +5477,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6387,7 +6384,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="I16:I18 C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6686,7 +6683,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6708,7 +6705,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6986,7 +6983,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="I16:I18 C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7285,7 +7282,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7307,7 +7304,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7581,7 +7578,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="I16:I18 C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7883,7 +7880,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7899,7 +7896,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>10</v>
@@ -8322,7 +8319,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="1" sqref="I16:I18 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8350,7 +8347,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>4</v>
@@ -8740,7 +8737,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8762,7 +8759,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>4</v>
@@ -9176,7 +9173,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="1" sqref="I16:I18 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9206,7 +9203,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>2</v>
@@ -9608,7 +9605,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9630,7 +9627,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>2</v>
@@ -10021,7 +10018,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="I16:I18 C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10508,7 +10505,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="1" sqref="I16:I18 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10540,7 +10537,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10951,7 +10948,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="1" sqref="I16:I18 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10982,7 +10979,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11390,7 +11387,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="1" sqref="I16:I18 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11409,7 +11406,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>3</v>
@@ -11835,7 +11832,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11857,7 +11854,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>10</v>
@@ -12272,7 +12269,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12294,7 +12291,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>2</v>
@@ -12717,7 +12714,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="1" sqref="I16:I18 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12745,7 +12742,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>2</v>
@@ -13162,7 +13159,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13184,7 +13181,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13463,7 +13460,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13485,7 +13482,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13762,7 +13759,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="1" sqref="I16:I18 I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14013,7 +14010,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="I16:I18 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14032,7 +14029,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14263,8 +14260,8 @@
   </sheetPr>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I16:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15158,7 +15155,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="I16:I18 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15186,7 +15183,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>2</v>
@@ -15589,7 +15586,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="I16:I18 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15614,7 +15611,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>11</v>
@@ -16029,7 +16026,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="I16:I18 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16054,7 +16051,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>2</v>
@@ -16469,7 +16466,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16488,7 +16485,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>10</v>
@@ -16894,7 +16891,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16913,7 +16910,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>4</v>
@@ -17334,7 +17331,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="I16:I18 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17359,7 +17356,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>2</v>
@@ -17774,7 +17771,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="I16:I18 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17802,7 +17799,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18214,7 +18211,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="I16:I18 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18230,7 +18227,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>11</v>
@@ -18654,7 +18651,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="I16:I18 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18682,7 +18679,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19094,7 +19091,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19107,7 +19104,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>2</v>
@@ -19534,7 +19531,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+      <selection pane="topLeft" activeCell="H30" activeCellId="1" sqref="I16:I18 H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20105,7 +20102,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="I16:I18 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20127,7 +20124,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>10</v>
@@ -20545,7 +20542,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="I16:I18 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20567,7 +20564,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>11</v>
@@ -20985,7 +20982,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21004,7 +21001,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>2</v>
@@ -21425,7 +21422,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="I16:I18 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21453,7 +21450,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21865,7 +21862,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21878,7 +21875,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>2</v>
@@ -22305,7 +22302,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22318,7 +22315,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>11</v>
@@ -22745,7 +22742,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22758,7 +22755,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>3</v>
@@ -23186,7 +23183,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I16:I18 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23199,7 +23196,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>2</v>
@@ -23625,8 +23622,8 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="1" sqref="I16:I18 D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23651,7 +23648,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>10</v>
@@ -24066,7 +24063,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="I16:I18 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24085,7 +24082,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>11</v>
@@ -24506,7 +24503,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="I16:I18 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25073,7 +25070,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="1" sqref="I16:I18 D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25786,7 +25783,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="I16:I18 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25805,7 +25802,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
@@ -26519,7 +26516,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+      <selection pane="topLeft" activeCell="G30" activeCellId="1" sqref="I16:I18 G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>